<commit_message>
move TNRSequencer, update my.SQL
</commit_message>
<xml_diff>
--- a/TNR/TCGenerator/TCGenerator_Article.xlsx
+++ b/TNR/TCGenerator/TCGenerator_Article.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="89">
   <si>
     <t>ID_CODGES</t>
   </si>
@@ -287,10 +287,7 @@
     <t>MAJ_MODFAM</t>
   </si>
   <si>
-    <t>DVID_NUMDOC1</t>
-  </si>
-  <si>
-    <t>????</t>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -442,228 +439,7 @@
     <cellStyle name="Normal 8" xfId="11"/>
     <cellStyle name="Normal 9" xfId="12"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1062,7 +838,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C18:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1442,20 +1218,21 @@
       <c r="B14" s="15" t="s">
         <v>88</v>
       </c>
+      <c r="C14" s="15"/>
       <c r="D14" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="F14" s="15" t="e">
+        <v>2</v>
+      </c>
+      <c r="F14" s="15" t="str">
         <f t="shared" si="10"/>
-        <v>#N/A</v>
-      </c>
-      <c r="G14" s="15" t="e">
+        <v>KW.scrollAndSetText(myJDD,"Notes")</v>
+      </c>
+      <c r="G14" s="15" t="str">
         <f t="shared" si="11"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H14" s="15" t="e">
+        <v>KW.scrollAndSetText(myJDD, "Notes")</v>
+      </c>
+      <c r="H14" s="15" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>KW.verifyValue(myJDD,"Notes")</v>
       </c>
       <c r="I14" s="17" t="str">
         <f t="shared" si="13"/>
@@ -1502,15 +1279,15 @@
       <c r="B17" s="14"/>
       <c r="D17" s="15"/>
       <c r="F17" s="15" t="str">
-        <f t="shared" ref="F17:F36" si="15">IF(ISBLANK(D17),"",VLOOKUP(D17,TAG_List,2,FALSE)&amp;B17&amp;VLOOKUP(D17,TAG_List,3,FALSE))</f>
+        <f t="shared" ref="F17:F35" si="15">IF(ISBLANK(D17),"",VLOOKUP(D17,TAG_List,2,FALSE)&amp;B17&amp;VLOOKUP(D17,TAG_List,3,FALSE))</f>
         <v/>
       </c>
       <c r="G17" s="15" t="str">
-        <f t="shared" ref="G17:G36" si="16">IF(ISBLANK(D17),"",VLOOKUP(D17,TAG_List,4,FALSE)&amp;B17&amp;VLOOKUP(D17,TAG_List,5,FALSE))</f>
+        <f t="shared" ref="G17:G35" si="16">IF(ISBLANK(D17),"",VLOOKUP(D17,TAG_List,4,FALSE)&amp;B17&amp;VLOOKUP(D17,TAG_List,5,FALSE))</f>
         <v/>
       </c>
       <c r="H17" s="15" t="str">
-        <f t="shared" ref="H17:H36" si="17">IF(ISBLANK(D17),"",VLOOKUP(D17,TAG_List,6,FALSE)&amp;B17&amp;VLOOKUP(D17,TAG_List,7,FALSE))</f>
+        <f t="shared" ref="H17:H35" si="17">IF(ISBLANK(D17),"",VLOOKUP(D17,TAG_List,6,FALSE)&amp;B17&amp;VLOOKUP(D17,TAG_List,7,FALSE))</f>
         <v/>
       </c>
       <c r="I17" s="17" t="str">
@@ -2206,10 +1983,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:H1048576">
-    <cfRule type="expression" dxfId="23" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$D1="block"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>$D1="onglet"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2231,7 +2008,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Gestion INTERNALVALUE déplacée de TNR/.Properties vers JDD.GLOABL
Traitement MAT en cours
</commit_message>
<xml_diff>
--- a/TNR/TCGenerator/TCGenerator_Article.xlsx
+++ b/TNR/TCGenerator/TCGenerator_Article.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="48" windowWidth="22116" windowHeight="11400" activeTab="2"/>
+    <workbookView xWindow="288" yWindow="48" windowWidth="22116" windowHeight="11400"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez moi" sheetId="5" r:id="rId1"/>
@@ -720,24 +720,7 @@
     <cellStyle name="Normal 8" xfId="11"/>
     <cellStyle name="Normal 9" xfId="12"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1081,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A6:E11"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1250,7 +1233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B40" sqref="B40:B55"/>
     </sheetView>
@@ -3280,26 +3263,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B35 B41:B1048576 C1:H1048576 A1:A1048576">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$D1="block"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>$D1="onglet"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:B37">
-    <cfRule type="expression" dxfId="5" priority="11">
+    <cfRule type="expression" dxfId="3" priority="11">
       <formula>$D37="block"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="12">
+    <cfRule type="expression" dxfId="2" priority="12">
       <formula>$D37="onglet"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="expression" dxfId="3" priority="19">
+    <cfRule type="expression" dxfId="1" priority="19">
       <formula>$D40="block"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="20">
+    <cfRule type="expression" dxfId="0" priority="20">
       <formula>$D40="onglet"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>